<commit_message>
revised course outcomes and synthetic student grades
</commit_message>
<xml_diff>
--- a/knowledge/course_outcomes_to_program_outcomes_mapping.xlsx
+++ b/knowledge/course_outcomes_to_program_outcomes_mapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rivieredu-my.sharepoint.com/personal/jglossner_rivier_edu/Documents/Courses/CS699 Professional Seminar/COMP 699 SP25/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siric\GitRivier\scthumma-assessment\knowledge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE6BCE86-A9B8-4440-BF37-41B083EEF954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F85EA63-939B-401B-8ABF-B8533A11523A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{54D4318A-BA62-4CE9-90EA-945AA24162DB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{54D4318A-BA62-4CE9-90EA-945AA24162DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -335,11 +335,29 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -347,28 +365,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -708,75 +708,75 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="16"/>
-      <c r="B1" s="18">
-        <v>180</v>
-      </c>
-      <c r="C1" s="18">
-        <v>181</v>
-      </c>
-      <c r="D1" s="18">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="26"/>
+      <c r="B1" s="24">
+        <v>101</v>
+      </c>
+      <c r="C1" s="24">
+        <v>103</v>
+      </c>
+      <c r="D1" s="24">
         <v>245</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="18">
+      <c r="F1" s="24">
         <v>301</v>
       </c>
-      <c r="G1" s="18">
+      <c r="G1" s="24">
         <v>308</v>
       </c>
-      <c r="H1" s="18">
+      <c r="H1" s="24">
         <v>315</v>
       </c>
-      <c r="I1" s="18">
+      <c r="I1" s="24">
         <v>335</v>
       </c>
-      <c r="J1" s="18">
+      <c r="J1" s="24">
         <v>385</v>
       </c>
-      <c r="K1" s="18">
+      <c r="K1" s="24">
         <v>405</v>
       </c>
-      <c r="L1" s="18">
+      <c r="L1" s="24">
         <v>430</v>
       </c>
-      <c r="M1" s="18">
+      <c r="M1" s="24">
         <v>450</v>
       </c>
-      <c r="N1" s="20">
+      <c r="N1" s="22">
         <v>495</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="27"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
       <c r="E2" s="2">
         <v>250</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="21"/>
-    </row>
-    <row r="3" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="23"/>
+    </row>
+    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -789,7 +789,7 @@
       <c r="D3" s="7">
         <v>2</v>
       </c>
-      <c r="E3" s="22"/>
+      <c r="E3" s="18"/>
       <c r="F3" s="7">
         <v>1</v>
       </c>
@@ -799,13 +799,13 @@
       <c r="H3" s="7">
         <v>1</v>
       </c>
-      <c r="I3" s="22">
+      <c r="I3" s="18">
         <v>1</v>
       </c>
       <c r="J3" s="7">
         <v>1</v>
       </c>
-      <c r="K3" s="22">
+      <c r="K3" s="18">
         <v>8</v>
       </c>
       <c r="L3" s="7">
@@ -818,7 +818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="180" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -831,7 +831,7 @@
       <c r="D4" s="7">
         <v>3</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="7">
         <v>2</v>
       </c>
@@ -841,11 +841,11 @@
       <c r="H4" s="7">
         <v>2</v>
       </c>
-      <c r="I4" s="23"/>
+      <c r="I4" s="19"/>
       <c r="J4" s="7">
         <v>4</v>
       </c>
-      <c r="K4" s="23"/>
+      <c r="K4" s="19"/>
       <c r="L4" s="7">
         <v>4</v>
       </c>
@@ -856,7 +856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="195" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -865,7 +865,7 @@
       <c r="D5" s="7">
         <v>4</v>
       </c>
-      <c r="E5" s="23"/>
+      <c r="E5" s="19"/>
       <c r="F5" s="7">
         <v>3</v>
       </c>
@@ -875,9 +875,9 @@
       <c r="H5" s="7">
         <v>3</v>
       </c>
-      <c r="I5" s="23"/>
+      <c r="I5" s="19"/>
       <c r="J5" s="8"/>
-      <c r="K5" s="23"/>
+      <c r="K5" s="19"/>
       <c r="L5" s="7">
         <v>5</v>
       </c>
@@ -886,20 +886,20 @@
       </c>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="23"/>
+      <c r="E6" s="19"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="7">
         <v>7</v>
       </c>
-      <c r="I6" s="23"/>
+      <c r="I6" s="19"/>
       <c r="J6" s="8"/>
-      <c r="K6" s="23"/>
+      <c r="K6" s="19"/>
       <c r="L6" s="7">
         <v>6</v>
       </c>
@@ -908,29 +908,29 @@
       </c>
       <c r="N6" s="8"/>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
-      <c r="E7" s="24"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="10">
         <v>8</v>
       </c>
-      <c r="I7" s="24"/>
+      <c r="I7" s="20"/>
       <c r="J7" s="9"/>
-      <c r="K7" s="24"/>
+      <c r="K7" s="20"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
     </row>
-    <row r="8" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="16">
         <v>4</v>
       </c>
       <c r="C8" s="11">
@@ -939,7 +939,7 @@
       <c r="D8" s="11">
         <v>1</v>
       </c>
-      <c r="E8" s="25"/>
+      <c r="E8" s="16"/>
       <c r="F8" s="11">
         <v>4</v>
       </c>
@@ -964,22 +964,22 @@
       <c r="M8" s="11">
         <v>1</v>
       </c>
-      <c r="N8" s="25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="240" x14ac:dyDescent="0.25">
+      <c r="N8" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="26"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="11">
         <v>4</v>
       </c>
       <c r="D9" s="11">
         <v>14</v>
       </c>
-      <c r="E9" s="26"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="11">
         <v>5</v>
       </c>
@@ -1004,18 +1004,18 @@
       <c r="M9" s="11">
         <v>4</v>
       </c>
-      <c r="N9" s="26"/>
-    </row>
-    <row r="10" spans="1:14" ht="270" x14ac:dyDescent="0.25">
+      <c r="N9" s="21"/>
+    </row>
+    <row r="10" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="26"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="11">
         <v>5</v>
       </c>
       <c r="D10" s="13"/>
-      <c r="E10" s="26"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="11">
         <v>6</v>
       </c>
@@ -1034,16 +1034,16 @@
         <v>5</v>
       </c>
       <c r="M10" s="13"/>
-      <c r="N10" s="26"/>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N10" s="21"/>
+    </row>
+    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6"/>
-      <c r="B11" s="27"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="12">
         <v>6</v>
       </c>
       <c r="D11" s="14"/>
-      <c r="E11" s="27"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -1056,213 +1056,213 @@
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
       <c r="M11" s="14"/>
-      <c r="N11" s="27"/>
-    </row>
-    <row r="12" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="N11" s="17"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="18">
         <v>3</v>
       </c>
       <c r="C12" s="7">
         <v>4</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22">
+      <c r="D12" s="18"/>
+      <c r="E12" s="18">
         <v>7</v>
       </c>
       <c r="F12" s="7">
         <v>5</v>
       </c>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22">
-        <v>6</v>
-      </c>
-      <c r="I12" s="22">
+      <c r="G12" s="18"/>
+      <c r="H12" s="18">
+        <v>6</v>
+      </c>
+      <c r="I12" s="18">
         <v>3</v>
       </c>
       <c r="J12" s="7">
         <v>6</v>
       </c>
-      <c r="K12" s="22">
+      <c r="K12" s="18">
         <v>7</v>
       </c>
-      <c r="L12" s="22"/>
+      <c r="L12" s="18"/>
       <c r="M12" s="7">
         <v>4</v>
       </c>
-      <c r="N12" s="22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="285.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N12" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="24"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="10">
         <v>5</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="10">
         <v>6</v>
       </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
       <c r="J13" s="10">
         <v>8</v>
       </c>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
       <c r="M13" s="10">
         <v>5</v>
       </c>
-      <c r="N13" s="24"/>
-    </row>
-    <row r="14" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="N13" s="20"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25">
-        <v>5</v>
-      </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25">
-        <v>4</v>
-      </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25">
+      <c r="B14" s="16"/>
+      <c r="C14" s="16">
+        <v>5</v>
+      </c>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16">
+        <v>4</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16">
         <v>8</v>
       </c>
       <c r="K14" s="11">
         <v>1</v>
       </c>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25">
+      <c r="L14" s="16"/>
+      <c r="M14" s="16">
         <v>9</v>
       </c>
       <c r="N14" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
       <c r="K15" s="11">
         <v>5</v>
       </c>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
       <c r="N15" s="11">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
       <c r="K16" s="12">
         <v>6</v>
       </c>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
       <c r="N16" s="14"/>
     </row>
-    <row r="17" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
       <c r="E17" s="7">
         <v>1</v>
       </c>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22">
+      <c r="F17" s="18"/>
+      <c r="G17" s="18">
         <v>9</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="18">
         <v>10</v>
       </c>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22">
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18">
         <v>9</v>
       </c>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22">
+      <c r="L17" s="18"/>
+      <c r="M17" s="18">
         <v>8</v>
       </c>
       <c r="N17" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="10">
         <v>4</v>
       </c>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
       <c r="N18" s="10">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="25"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="11">
         <v>3</v>
       </c>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25">
-        <v>2</v>
-      </c>
-      <c r="F19" s="25">
+      <c r="D19" s="16"/>
+      <c r="E19" s="16">
+        <v>2</v>
+      </c>
+      <c r="F19" s="16">
         <v>6</v>
       </c>
       <c r="G19" s="11">
         <v>1</v>
       </c>
-      <c r="H19" s="25"/>
+      <c r="H19" s="16"/>
       <c r="I19" s="11">
         <v>3</v>
       </c>
@@ -1282,21 +1282,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="26"/>
+      <c r="B20" s="21"/>
       <c r="C20" s="11">
         <v>6</v>
       </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
       <c r="G20" s="11">
         <v>4</v>
       </c>
-      <c r="H20" s="26"/>
+      <c r="H20" s="21"/>
       <c r="I20" s="11">
         <v>5</v>
       </c>
@@ -1316,19 +1316,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="27"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="14"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
       <c r="G21" s="12">
         <v>9</v>
       </c>
-      <c r="H21" s="27"/>
+      <c r="H21" s="17"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
       <c r="K21" s="12">
@@ -1344,27 +1344,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22">
-        <v>6</v>
-      </c>
-      <c r="D22" s="22"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18">
+        <v>6</v>
+      </c>
+      <c r="D22" s="18"/>
       <c r="E22" s="7">
         <v>2</v>
       </c>
-      <c r="F22" s="22"/>
+      <c r="F22" s="18"/>
       <c r="G22" s="7">
         <v>8</v>
       </c>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22">
-        <v>6</v>
-      </c>
-      <c r="J22" s="22">
+      <c r="H22" s="18"/>
+      <c r="I22" s="18">
+        <v>6</v>
+      </c>
+      <c r="J22" s="18">
         <v>9</v>
       </c>
       <c r="K22" s="7">
@@ -1380,23 +1380,23 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
       <c r="E23" s="7">
         <v>7</v>
       </c>
-      <c r="F23" s="23"/>
+      <c r="F23" s="19"/>
       <c r="G23" s="7">
         <v>9</v>
       </c>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
       <c r="K23" s="7">
         <v>5</v>
       </c>
@@ -1410,19 +1410,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
       <c r="E24" s="8"/>
-      <c r="F24" s="23"/>
+      <c r="F24" s="19"/>
       <c r="G24" s="8"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
       <c r="K24" s="8"/>
       <c r="L24" s="7">
         <v>12</v>
@@ -1432,113 +1432,93 @@
       </c>
       <c r="N24" s="7"/>
     </row>
-    <row r="25" spans="1:14" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
       <c r="E25" s="9"/>
-      <c r="F25" s="24"/>
+      <c r="F25" s="20"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
       <c r="K25" s="9"/>
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
       <c r="N25" s="9"/>
     </row>
-    <row r="26" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25">
+      <c r="B26" s="16"/>
+      <c r="C26" s="16">
         <v>7</v>
       </c>
-      <c r="D26" s="25"/>
+      <c r="D26" s="16"/>
       <c r="E26" s="11">
         <v>3</v>
       </c>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25">
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16">
         <v>9</v>
       </c>
-      <c r="L26" s="25"/>
-      <c r="M26" s="25">
+      <c r="L26" s="16"/>
+      <c r="M26" s="16">
         <v>8</v>
       </c>
-      <c r="N26" s="25">
+      <c r="N26" s="16">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
       <c r="E27" s="12">
         <v>9</v>
       </c>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="27"/>
-      <c r="N27" s="27"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="N26:N27"/>
-    <mergeCell ref="J22:J25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="F22:F25"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="I22:I25"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="H19:H21"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="J14:J16"/>
-    <mergeCell ref="L14:L16"/>
-    <mergeCell ref="M14:M16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="E3:E7"/>
+    <mergeCell ref="I3:I7"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="N8:N11"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="G1:G2"/>
     <mergeCell ref="K12:K13"/>
     <mergeCell ref="L12:L13"/>
     <mergeCell ref="N12:N13"/>
@@ -1555,25 +1535,45 @@
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="H12:H13"/>
     <mergeCell ref="I12:I13"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="E3:E7"/>
-    <mergeCell ref="I3:I7"/>
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="N8:N11"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="L14:L16"/>
+    <mergeCell ref="M14:M16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="H19:H21"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="F22:F25"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="I22:I25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="N26:N27"/>
+    <mergeCell ref="J22:J25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>